<commit_message>
Automation Toolkit Release v9.2.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA856E9-3FA5-F84B-A1F4-432EE88715BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A26D7FD-8015-B646-9832-D3FA24C7F28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16220" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -3897,211 +3897,6 @@
     <t>INGRESS</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Tool Kit does not support Export or Creation of Instances with multiple VNICs currently.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-"Pub Address" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Represents whether public address needs to be assigned to the instance or not(TRUE|FALSE).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"SSH Key Var Name" -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Accepts SSH Key value or the name of the variable defined in variables_&lt;region&gt;.tf file containing SSH key; Multiple keys should be separated by \n
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NSGs" -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG.
-"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DedicatedVMHost" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Leave this field empty if the instance does not need to be launched on dedicated vm host.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Source Details" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Specify if the instance is to be launched from Image or Boot Volume.
-                                    Format - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>image::&lt;variable containing image ocid&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (or)  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bootVolume::&lt;variable  containing boot volume ocid&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>DRG Name</t>
   </si>
   <si>
@@ -6167,12 +5962,255 @@
   <si>
     <t>ADB workload</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Tool Kit does not support Export or Creation of Instances with multiple VNICs currently. CD3 Automation toolkit will not export instances launched by OKE.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Pub Address" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Represents whether public address needs to be assigned to the instance or not(TRUE|FALSE).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"SSH Key Var Name" -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Accepts SSH Key value or the name of the variable defined in variables_&lt;region&gt;.tf file containing SSH key; Multiple keys should be separated by \n
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NSGs" -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG.
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DedicatedVMHost" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Leave this field empty if the instance does not need to be launched on dedicated vm host.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Source Details" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Specify if the instance is to be launched from Image or Boot Volume.
+                                    Format - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image::&lt;variable containing image ocid&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (or) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>image::&lt;variable containing the market place image name</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (or)  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bootVolume::&lt;variable  containing boot volume ocid&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6394,6 +6432,11 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
@@ -11194,7 +11237,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -16021,7 +16064,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -16041,25 +16084,25 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>414</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>415</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>44</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>269</v>
@@ -16647,7 +16690,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="31" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>411</v>
+        <v>566</v>
       </c>
       <c r="B1" s="90"/>
       <c r="C1" s="90"/>
@@ -16657,7 +16700,7 @@
       <c r="G1" s="90"/>
       <c r="H1" s="91"/>
       <c r="I1" s="81" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J1" s="82"/>
       <c r="K1" s="82"/>
@@ -16703,16 +16746,16 @@
         <v>67</v>
       </c>
       <c r="K2" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>530</v>
       </c>
-      <c r="L2" s="28" t="s">
-        <v>531</v>
-      </c>
       <c r="M2" s="29" t="s">
+        <v>534</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>535</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>536</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>72</v>
@@ -16861,10 +16904,10 @@
         <v>83</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>73</v>
@@ -17135,13 +17178,13 @@
         <v>99</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>419</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>420</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>100</v>
@@ -17153,7 +17196,7 @@
         <v>74</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>102</v>
@@ -17326,7 +17369,7 @@
   <sheetData>
     <row r="1" spans="1:22" s="31" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -17361,16 +17404,16 @@
         <v>99</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F2" s="33" t="s">
         <v>110</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>111</v>
@@ -17492,7 +17535,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="31" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -17534,10 +17577,10 @@
         <v>165</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J2" s="29" t="s">
         <v>166</v>
@@ -17833,7 +17876,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -17855,19 +17898,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>166</v>
@@ -17876,7 +17919,7 @@
         <v>110</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="K2" s="29" t="s">
         <v>167</v>
@@ -18214,7 +18257,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -18235,19 +18278,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="29" t="s">
+        <v>549</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>550</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="G2" s="29" t="s">
         <v>551</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>552</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>113</v>
@@ -18259,7 +18302,7 @@
         <v>296</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -18313,7 +18356,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -18339,34 +18382,34 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>217</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H2" s="79" t="s">
         <v>218</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>561</v>
+      </c>
+      <c r="K2" s="18" t="s">
         <v>562</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>563</v>
-      </c>
       <c r="L2" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="M2" s="49" t="s">
         <v>223</v>
@@ -18515,31 +18558,31 @@
         <v>29</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="49" t="s">
+        <v>483</v>
+      </c>
+      <c r="H2" s="49" t="s">
         <v>484</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="I2" s="49" t="s">
         <v>485</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="J2" s="49" t="s">
         <v>486</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="K2" s="64" t="s">
         <v>487</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="L2" s="49" t="s">
         <v>488</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="M2" s="50" t="s">
         <v>489</v>
-      </c>
-      <c r="M2" s="50" t="s">
-        <v>490</v>
       </c>
       <c r="N2" s="49" t="s">
         <v>256</v>
@@ -18557,10 +18600,10 @@
         <v>259</v>
       </c>
       <c r="S2" s="49" t="s">
+        <v>490</v>
+      </c>
+      <c r="T2" s="49" t="s">
         <v>491</v>
-      </c>
-      <c r="T2" s="49" t="s">
-        <v>492</v>
       </c>
       <c r="U2" s="49" t="s">
         <v>72</v>
@@ -18572,7 +18615,7 @@
         <v>224</v>
       </c>
       <c r="X2" s="49" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Y2" s="49" t="s">
         <v>405</v>
@@ -24617,7 +24660,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -24635,7 +24678,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D2" s="64" t="s">
         <v>66</v>
@@ -24644,10 +24687,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="64" t="s">
+        <v>503</v>
+      </c>
+      <c r="G2" s="64" t="s">
         <v>504</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>505</v>
       </c>
       <c r="H2" s="67" t="s">
         <v>269</v>
@@ -30721,34 +30764,34 @@
         <v>6</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D2" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="E2" s="64" t="s">
         <v>508</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>509</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>239</v>
       </c>
       <c r="G2" s="64" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I2" s="64" t="s">
         <v>256</v>
       </c>
       <c r="J2" s="64" t="s">
+        <v>509</v>
+      </c>
+      <c r="K2" s="64" t="s">
         <v>510</v>
       </c>
-      <c r="K2" s="64" t="s">
+      <c r="L2" s="64" t="s">
         <v>511</v>
-      </c>
-      <c r="L2" s="64" t="s">
-        <v>512</v>
       </c>
       <c r="M2" s="64" t="s">
         <v>72</v>
@@ -30760,7 +30803,7 @@
         <v>74</v>
       </c>
       <c r="P2" s="74" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="Q2" s="71" t="s">
         <v>269</v>
@@ -37657,22 +37700,22 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>263</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E1" s="40" t="s">
         <v>241</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>224</v>
@@ -37681,16 +37724,16 @@
         <v>223</v>
       </c>
       <c r="I1" s="66" t="s">
+        <v>487</v>
+      </c>
+      <c r="J1" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="J1" s="66" t="s">
-        <v>489</v>
-      </c>
       <c r="K1" s="46" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -37722,7 +37765,7 @@
         <v>80</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K2" s="32">
         <v>1</v>
@@ -37733,7 +37776,7 @@
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="65" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>265</v>
@@ -37760,7 +37803,7 @@
         <v>40</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K3" s="32">
         <v>2</v>
@@ -37771,7 +37814,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>237</v>
@@ -37788,7 +37831,7 @@
         <v>298</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -37796,7 +37839,7 @@
         <v>233</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>266</v>
@@ -37810,7 +37853,7 @@
         <v>299</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -37819,7 +37862,7 @@
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32" t="s">
@@ -37832,11 +37875,11 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="65" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32" t="s">
@@ -37849,11 +37892,11 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="65" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B8" s="32"/>
       <c r="C8" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="32" t="s">
@@ -37887,7 +37930,7 @@
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32" t="s">
@@ -37900,11 +37943,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="65" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32" t="s">
@@ -37921,11 +37964,11 @@
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F12" s="32"/>
       <c r="H12" s="32" t="s">
@@ -37938,7 +37981,7 @@
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
@@ -37953,7 +37996,7 @@
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -38487,91 +38530,91 @@
   <sheetData>
     <row r="1" spans="1:39" s="54" customFormat="1" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
+        <v>420</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>421</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="C1" s="62" t="s">
         <v>422</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="D1" s="62" t="s">
         <v>423</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="E1" s="62" t="s">
         <v>424</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="F1" s="62" t="s">
         <v>425</v>
-      </c>
-      <c r="F1" s="62" t="s">
-        <v>426</v>
       </c>
       <c r="G1" s="62" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="62" t="s">
+        <v>426</v>
+      </c>
+      <c r="I1" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="J1" s="62" t="s">
         <v>428</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>429</v>
       </c>
-      <c r="K1" s="62" t="s">
+      <c r="L1" s="62" t="s">
         <v>430</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="M1" s="62" t="s">
+        <v>478</v>
+      </c>
+      <c r="N1" s="62" t="s">
         <v>431</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="O1" s="62" t="s">
+        <v>432</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q1" s="62" t="s">
+        <v>434</v>
+      </c>
+      <c r="R1" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="S1" s="62" t="s">
+        <v>436</v>
+      </c>
+      <c r="T1" s="62" t="s">
+        <v>480</v>
+      </c>
+      <c r="U1" s="62" t="s">
+        <v>437</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>438</v>
+      </c>
+      <c r="W1" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y1" s="62" t="s">
         <v>479</v>
-      </c>
-      <c r="N1" s="62" t="s">
-        <v>432</v>
-      </c>
-      <c r="O1" s="62" t="s">
-        <v>433</v>
-      </c>
-      <c r="P1" s="62" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q1" s="62" t="s">
-        <v>435</v>
-      </c>
-      <c r="R1" s="62" t="s">
-        <v>436</v>
-      </c>
-      <c r="S1" s="62" t="s">
-        <v>437</v>
-      </c>
-      <c r="T1" s="62" t="s">
-        <v>481</v>
-      </c>
-      <c r="U1" s="62" t="s">
-        <v>438</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>439</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>440</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>441</v>
-      </c>
-      <c r="Y1" s="62" t="s">
-        <v>480</v>
       </c>
       <c r="Z1" s="53" t="s">
         <v>67</v>
       </c>
       <c r="AA1" s="53" t="s">
+        <v>441</v>
+      </c>
+      <c r="AB1" s="53" t="s">
         <v>442</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AC1" s="53" t="s">
         <v>443</v>
-      </c>
-      <c r="AC1" s="53" t="s">
-        <v>444</v>
       </c>
       <c r="AD1" s="53" t="s">
         <v>169</v>
@@ -38592,7 +38635,7 @@
         <v>174</v>
       </c>
       <c r="AJ1" s="53" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AK1" s="53" t="s">
         <v>219</v>
@@ -38624,7 +38667,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H2" s="56" t="s">
         <v>28</v>
@@ -38653,7 +38696,7 @@
         <v>63</v>
       </c>
       <c r="P2" s="57" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Q2" s="56" t="s">
         <v>248</v>
@@ -38673,13 +38716,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="56" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="W2" s="56" t="s">
         <v>98</v>
       </c>
       <c r="X2" s="56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Y2" s="56" t="b">
         <v>1</v>
@@ -38688,7 +38731,7 @@
         <v>108</v>
       </c>
       <c r="AA2" s="56" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AB2" s="56" t="s">
         <v>122</v>
@@ -38783,7 +38826,7 @@
         <v>69</v>
       </c>
       <c r="S3" s="56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="T3" s="56" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A3,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A3,3,4,1,"DedicatedVMHosts")))</f>
@@ -38800,7 +38843,7 @@
         <v>97</v>
       </c>
       <c r="X3" s="56" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Y3" s="56" t="b">
         <v>0</v>
@@ -38812,7 +38855,7 @@
         <v>121</v>
       </c>
       <c r="AB3" s="56" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AC3" s="56" t="s">
         <v>123</v>
@@ -38836,7 +38879,7 @@
         <v>16</v>
       </c>
       <c r="AJ3" s="56" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AK3" s="55" t="s">
         <v>222</v>
@@ -38864,7 +38907,7 @@
       </c>
       <c r="F4" s="56"/>
       <c r="G4" s="56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="56" t="s">
@@ -38894,7 +38937,7 @@
         <v>76</v>
       </c>
       <c r="S4" s="56" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="T4" s="56" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">IF(COUNTIF(INDIRECT(ADDRESS(3,1,1,1,"DedicatedVMHosts")&amp;":"&amp;ADDRESS(A4,1,4,1)),"*END*")&gt;0,"",INDIRECT(ADDRESS(A4,3,4,1,"DedicatedVMHosts")))</f>
@@ -38907,14 +38950,14 @@
       <c r="V4" s="56"/>
       <c r="W4" s="56"/>
       <c r="X4" s="56" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="56" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA4" s="56" t="s">
         <v>457</v>
-      </c>
-      <c r="AA4" s="56" t="s">
-        <v>458</v>
       </c>
       <c r="AB4" s="56"/>
       <c r="AC4" s="56" t="s">
@@ -38961,7 +39004,7 @@
       </c>
       <c r="F5" s="56"/>
       <c r="G5" s="56" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H5" s="56"/>
       <c r="I5" s="56" t="s">
@@ -38979,7 +39022,7 @@
       </c>
       <c r="N5" s="56"/>
       <c r="O5" s="56" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P5" s="57"/>
       <c r="Q5" s="56"/>
@@ -38996,7 +39039,7 @@
       <c r="X5" s="56"/>
       <c r="Y5" s="56"/>
       <c r="Z5" s="56" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AA5" s="56"/>
       <c r="AB5" s="56"/>
@@ -39040,7 +39083,7 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H6" s="56"/>
       <c r="I6" s="56"/>
@@ -39111,7 +39154,7 @@
       </c>
       <c r="F7" s="56"/>
       <c r="G7" s="56" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H7" s="56"/>
       <c r="I7" s="56"/>
@@ -39180,7 +39223,7 @@
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="56" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
@@ -39249,7 +39292,7 @@
       </c>
       <c r="F9" s="56"/>
       <c r="G9" s="56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
@@ -39318,7 +39361,7 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
@@ -39387,7 +39430,7 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="56" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
@@ -39456,7 +39499,7 @@
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H12" s="56"/>
       <c r="I12" s="56"/>
@@ -39523,7 +39566,7 @@
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
@@ -39590,7 +39633,7 @@
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H14" s="56"/>
       <c r="I14" s="56"/>
@@ -39724,7 +39767,7 @@
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
@@ -39791,7 +39834,7 @@
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="56" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
@@ -39858,7 +39901,7 @@
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="56" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
@@ -39925,7 +39968,7 @@
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="56" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
@@ -39992,7 +40035,7 @@
       </c>
       <c r="F20" s="56"/>
       <c r="G20" s="56" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
@@ -40059,7 +40102,7 @@
       </c>
       <c r="F21" s="56"/>
       <c r="G21" s="56" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
@@ -40126,7 +40169,7 @@
       </c>
       <c r="F22" s="56"/>
       <c r="G22" s="56" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
@@ -40193,7 +40236,7 @@
       </c>
       <c r="F23" s="56"/>
       <c r="G23" s="56" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
@@ -40260,7 +40303,7 @@
       </c>
       <c r="F24" s="56"/>
       <c r="G24" s="56" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
@@ -42033,10 +42076,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -42599,7 +42642,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -42607,7 +42650,7 @@
       <c r="E1" s="82"/>
       <c r="F1" s="83"/>
       <c r="G1" s="84" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H1" s="85"/>
       <c r="I1" s="85"/>
@@ -42638,7 +42681,7 @@
         <v>215</v>
       </c>
       <c r="I2" s="36" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="52" customFormat="1" x14ac:dyDescent="0.2">
@@ -42775,7 +42818,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -42802,7 +42845,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -42894,14 +42937,14 @@
   <sheetData>
     <row r="1" spans="1:8" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
       <c r="D1" s="80"/>
       <c r="E1" s="80"/>
       <c r="F1" s="86" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G1" s="86"/>
       <c r="H1" s="86"/>
@@ -42914,19 +42957,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="F2" s="78" t="s">
         <v>414</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="G2" s="29" t="s">
         <v>415</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>416</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>269</v>
@@ -42984,7 +43027,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="37" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B1" s="87"/>
     </row>
@@ -42998,19 +43041,19 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B5" s="32"/>
     </row>

</xml_diff>

<commit_message>
Automation Toolkit Release v10.2
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\cd3_automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F44BFA2-C6D7-4DC1-B543-23CDFF6FCC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3E301B-E6D6-4381-9803-DCA1FB5F3F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17113,7 +17113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -17137,7 +17137,7 @@
     <col min="19" max="19" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="137" customHeight="1">
+    <row r="1" spans="1:20" ht="155" customHeight="1">
       <c r="A1" s="80" t="s">
         <v>586</v>
       </c>

</xml_diff>

<commit_message>
Automation Toolkit Release v11.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\orahub_develop\cd3_automation_toolkit\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C57369-2067-42E9-BABF-B3BBD05AC0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A05C1F3-A7B8-4550-8C41-95FF589D3B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <sheet name="LB-Listener" sheetId="20" r:id="rId26"/>
     <sheet name="LB-RuleSet" sheetId="18" r:id="rId27"/>
     <sheet name="LB-PathRouteSet" sheetId="19" r:id="rId28"/>
-    <sheet name="NLB-Listeners " sheetId="57" r:id="rId29"/>
+    <sheet name="NLB-Listeners" sheetId="57" r:id="rId29"/>
     <sheet name="NLB-BackendSets-BackendServers" sheetId="35" r:id="rId30"/>
     <sheet name="ADB" sheetId="38" r:id="rId31"/>
     <sheet name="DBSystems-VM-BM" sheetId="24" r:id="rId32"/>

</xml_diff>

<commit_message>
Automation Toolkit Release v12
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/mycd3/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D36DD1-E727-0D4F-BCE3-21A4CD472600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFF09B6-BC06-7C49-BC20-05847C9A72CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13520" yWindow="760" windowWidth="16720" windowHeight="17540" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13520" yWindow="760" windowWidth="16720" windowHeight="17480" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -7294,57 +7294,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-"SDDC name" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Name of the SDDC
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Defined Tags" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
-                             </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example: Operations.CostCenter=01;Users.Name=user01</t>
-    </r>
-  </si>
-  <si>
     <t>SDDC Name</t>
   </si>
   <si>
@@ -8868,12 +8817,177 @@
   <si>
     <t>Workload Block Volumes</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+"SDDC name" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Name of the SDDC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Management Block Volumes" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Existing Block Volume Name (minimum - 8 TB ~ 8192 GB). Format - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip block_compartment if it is same as SDDC comaprtment.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Workload Block Volumes" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Existing Block Volume Names separated by ','. Format - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;,  &lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip block_compartment if it is same as SDDC compartment.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Defined Tags" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+                             Example: Operations.CostCenter=01;Users.Name=user01</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+** Management and Workload block volumes are needed only if SDDC is of Standard Shape.
+** Standard shapes aren't compatible with Monthly billing interval commitment and advanced HCX license types.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9174,8 +9288,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9232,6 +9362,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8CCE4"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -9434,7 +9570,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9630,6 +9766,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -9703,11 +9845,14 @@
     <xf numFmtId="0" fontId="33" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -14917,7 +15062,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -14942,10 +15087,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="34" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>512</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -15006,16 +15151,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="103.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" s="34" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -15087,31 +15232,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>653</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="89" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="91" t="s">
         <v>654</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
     </row>
     <row r="2" spans="1:21" s="34" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -20023,18 +20168,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>656</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
     </row>
     <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -20102,17 +20247,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>657</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -20176,25 +20321,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>658</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -20286,28 +20431,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -20405,17 +20550,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>660</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -20737,19 +20882,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>667</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
     </row>
     <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -20855,15 +21000,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:7" s="34" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -20917,13 +21062,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>647</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -20989,32 +21134,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="226" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
-        <v>716</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="82" t="s">
-        <v>722</v>
-      </c>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="84"/>
+      <c r="A1" s="95" t="s">
+        <v>715</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="84" t="s">
+        <v>721</v>
+      </c>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="86"/>
     </row>
     <row r="2" spans="1:22" s="34" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -21117,22 +21262,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>677</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
     </row>
     <row r="2" spans="1:14" s="34" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -21216,27 +21361,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="98" t="s">
         <v>679</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="101" t="s">
         <v>275</v>
       </c>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
-      <c r="N1" s="99"/>
-      <c r="O1" s="99"/>
-      <c r="P1" s="99"/>
-      <c r="Q1" s="99"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -21346,40 +21491,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>558</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="93" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="95" t="s">
         <v>680</v>
       </c>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="94"/>
-      <c r="Y1" s="94"/>
-      <c r="Z1" s="94"/>
-      <c r="AA1" s="94"/>
-      <c r="AB1" s="94"/>
-      <c r="AC1" s="94"/>
-      <c r="AD1" s="95"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
+      <c r="AA1" s="96"/>
+      <c r="AB1" s="96"/>
+      <c r="AC1" s="96"/>
+      <c r="AD1" s="97"/>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -21512,27 +21657,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>681</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
     </row>
     <row r="2" spans="1:19" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -21630,30 +21775,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>682</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="86"/>
     </row>
     <row r="2" spans="1:22" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
@@ -21757,25 +21902,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>519</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
     </row>
     <row r="2" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -21868,29 +22013,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="85" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="101"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="103"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -21980,14 +22125,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="34" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>683</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
     </row>
     <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -22044,21 +22189,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
     </row>
     <row r="2" spans="1:19" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -22413,13 +22558,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
-        <v>720</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
+      <c r="A1" s="81" t="s">
+        <v>719</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -22471,19 +22616,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
     </row>
     <row r="2" spans="1:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -22553,24 +22698,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="160" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>684</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
     </row>
     <row r="2" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -22684,35 +22829,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>685</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="85"/>
+      <c r="AA1" s="86"/>
     </row>
     <row r="2" spans="1:27" s="41" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
@@ -25801,16 +25946,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>686</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
@@ -28644,29 +28789,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
       <c r="V1" s="61"/>
       <c r="W1" s="61"/>
       <c r="X1" s="61"/>
@@ -28703,16 +28848,16 @@
         <v>490</v>
       </c>
       <c r="K2" s="55" t="s">
+        <v>722</v>
+      </c>
+      <c r="L2" s="55" t="s">
         <v>723</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="M2" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="N2" s="55" t="s">
         <v>725</v>
-      </c>
-      <c r="N2" s="55" t="s">
-        <v>726</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>491</v>
@@ -32974,25 +33119,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
-        <v>688</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
+      <c r="A1" s="108" t="s">
+        <v>728</v>
+      </c>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="110"/>
     </row>
     <row r="2" spans="1:17" s="41" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -33002,43 +33147,43 @@
         <v>6</v>
       </c>
       <c r="C2" s="27" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2" s="64" t="s">
         <v>689</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="E2" s="64" t="s">
         <v>690</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="F2" s="27" t="s">
         <v>691</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="64" t="s">
         <v>692</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="H2" s="27" t="s">
         <v>693</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>694</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>695</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="79" t="s">
+        <v>726</v>
+      </c>
+      <c r="L2" s="80" t="s">
+        <v>727</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>696</v>
       </c>
-      <c r="K2" s="106" t="s">
-        <v>727</v>
-      </c>
-      <c r="L2" s="107" t="s">
-        <v>728</v>
-      </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>697</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>698</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>699</v>
       </c>
       <c r="P2" s="27" t="s">
         <v>72</v>
@@ -33087,65 +33232,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
-        <v>700</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
+      <c r="A1" s="95" t="s">
+        <v>699</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
     </row>
     <row r="2" spans="1:15" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C2" s="64" t="s">
+        <v>700</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>701</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="27" t="s">
         <v>702</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="27" t="s">
         <v>703</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>704</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>705</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>706</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>707</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="27" t="s">
         <v>708</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>709</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>710</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>711</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>712</v>
       </c>
       <c r="O2" s="41"/>
     </row>
@@ -33200,26 +33345,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="261" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="103" t="s">
-        <v>713</v>
-      </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="105"/>
+      <c r="A1" s="105" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="107"/>
     </row>
     <row r="2" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -36216,15 +36361,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="34" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>648</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="83"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -37604,14 +37749,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="34" customFormat="1" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
-        <v>719</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="81"/>
+      <c r="A1" s="81" t="s">
+        <v>718</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -37624,10 +37769,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>269</v>
@@ -39202,16 +39347,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="34" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>649</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -41547,19 +41692,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="85" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="87" t="s">
         <v>650</v>
       </c>
-      <c r="H1" s="86"/>
-      <c r="I1" s="87"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
@@ -41626,22 +41771,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>651</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="82" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="84" t="s">
         <v>652</v>
       </c>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="84"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="1:12" s="34" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -41717,19 +41862,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>529</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="88" t="s">
-        <v>714</v>
-      </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="90" t="s">
+        <v>713</v>
+      </c>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -41745,7 +41890,7 @@
         <v>396</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
Automation Toolkit Release v12.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/cd3devrel/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/mycd3/cd3-automation-toolkit/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B509BD-4EE8-F449-ACF8-D28811A5A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5616E6A0-8BAD-7541-A989-BB78E6606840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Automation Toolkit Release v24.1.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0226742C-CDBF-EA49-9C8B-C603A542B798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1ADEE-DA6D-F442-B956-1F34A17B68F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6360" yWindow="1520" windowWidth="30240" windowHeight="17600" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -8409,48 +8409,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CD3 Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Release - v12
-Introduced new service - Network Sources, 
-Enhancements - Added support for multiple Exa VM Clusters, OCVS Standard Shapes, 
-NLB fix, Instance Terraform
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
 If the shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::&lt;ocpus&gt;
 "Create_Is PV Encryption In Transit Enabled" </t>
@@ -8984,6 +8942,44 @@
   </si>
   <si>
     <t>Plugin Vulnerability Scanning</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CD3-OCI Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Release - v2024.1.0</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -15065,7 +15061,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
     </row>
   </sheetData>
@@ -21146,7 +21142,7 @@
       <c r="G1" s="96"/>
       <c r="H1" s="97"/>
       <c r="I1" s="84" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J1" s="85"/>
       <c r="K1" s="85"/>
@@ -21207,7 +21203,7 @@
         <v>514</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>72</v>
@@ -28852,16 +28848,16 @@
         <v>490</v>
       </c>
       <c r="K2" s="55" t="s">
+        <v>721</v>
+      </c>
+      <c r="L2" s="55" t="s">
         <v>722</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="M2" s="55" t="s">
         <v>723</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="N2" s="55" t="s">
         <v>724</v>
-      </c>
-      <c r="N2" s="55" t="s">
-        <v>725</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>491</v>
@@ -33124,7 +33120,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="105" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="106"/>
@@ -33175,10 +33171,10 @@
         <v>695</v>
       </c>
       <c r="K2" s="79" t="s">
+        <v>725</v>
+      </c>
+      <c r="L2" s="80" t="s">
         <v>726</v>
-      </c>
-      <c r="L2" s="80" t="s">
-        <v>727</v>
       </c>
       <c r="M2" s="27" t="s">
         <v>696</v>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.2.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1ADEE-DA6D-F442-B956-1F34A17B68F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB805BCE-622F-2F44-A82C-4F4E426851CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1520" windowWidth="30240" windowHeight="17600" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -8957,7 +8957,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CD3-OCI Automation Toolkit</t>
+      <t>CD3 Automation Toolkit</t>
     </r>
     <r>
       <rPr>
@@ -8978,7 +8978,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Release - v2024.1.0</t>
+      <t>Release - v2024.2.0</t>
     </r>
   </si>
 </sst>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.2.1
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/CD3Lasya/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB805BCE-622F-2F44-A82C-4F4E426851CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA9B7FA-9A14-1F43-8658-37ECF92DBFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16040" windowHeight="17640" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -15045,7 +15045,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="0"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -15072,10 +15072,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15131,6 +15134,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -15201,10 +15207,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:T483"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20143,10 +20152,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20224,10 +20236,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20299,10 +20314,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20404,10 +20422,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView zoomScale="91" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20527,10 +20548,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F12FA-08B6-DD41-A702-ABBC64AAAA55}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20858,10 +20882,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FF5E6C-AFB2-B34B-881D-6B69B8DC5062}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20980,10 +21007,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21043,10 +21073,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21099,10 +21132,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21242,10 +21278,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21334,10 +21373,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView zoomScale="89" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21451,6 +21493,9 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EF99B6-A34F-624E-9962-B07C78FC3BD7}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -21634,10 +21679,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:S1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21752,10 +21800,13 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection sqref="A1:V1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21882,10 +21933,13 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21989,10 +22043,13 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22110,10 +22167,13 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22167,10 +22227,13 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7F0FCC-1E37-7145-B88D-B9F0D1AABC09}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22542,10 +22605,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22597,10 +22663,13 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F032E3C-E5A2-3544-A693-CF15A37770BF}">
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22678,10 +22747,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB95AE4A-F9E4-134A-864A-9F24C8E929EA}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22801,10 +22873,13 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:AA993"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25929,10 +26004,13 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:H921"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28753,10 +28831,13 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:AB995"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="78" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33103,10 +33184,13 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93ED903B-F69B-8440-8195-68F92D10C778}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33215,10 +33299,13 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA2CEDE1-096D-3A48-B241-B55C70848C6F}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33316,6 +33403,9 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047E11E2-D3E5-4BD8-BB43-57A57B87349F}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -36344,10 +36434,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999B7604-8A91-4603-BC51-D587A22D6DD8}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37734,6 +37827,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6790755E-B3EC-4AF9-B8F2-0E8E6A199B83}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39329,10 +39425,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:I230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41672,6 +41771,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41750,6 +41852,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41841,6 +41946,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.2.2
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/CD3Lasya/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA9B7FA-9A14-1F43-8658-37ECF92DBFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D17F91-55B4-A846-B06D-4423DEB347CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16040" windowHeight="17640" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -3696,164 +3696,6 @@
     <t>Node Defined Tags</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Allowed values for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Network Type" - FLANNEL_OVERLAY </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OCI_VCN_IP_NATIVE
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Enter subnet name as :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;vcn-name&gt;_&lt;subnet-name&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">or the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ocid
-"API Endpoint Pub Address" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Represents whether public address needs to be assigned to the control plane or not(TRUE|FALSE).</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-"SSH Key Var Name" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Accepts SSH Key value or the name of the variable defined in variables_&lt;region&gt;.tf file containing SSH key; Multiple keys should be separated by \n</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Columns with nsgs accept comma seperated list of NSG names or ocids that needs to be part of the particular component, leave it blank if it doesnot need to be part of any NSG. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>FLANNEL_OVERLAY</t>
   </si>
   <si>
@@ -7888,8 +7730,552 @@
     <t>RPC Display Name</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+    <t>OCI Networks</t>
+  </si>
+  <si>
+    <t>Public Networks</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
+"Name" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Name) is a mandatory field.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Description" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Description) is a mandatory field.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Public Networks" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">It is an optional field. Specify comma separated list of public CIDRs to be included.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"OCI Networks" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">It is an optional field. Format: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specify comma separated list of VCN CIDR to be included. For ex:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">10.0.2.0/18,10.0.3.0/18
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Defined Tags" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
+                                </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example: Operations.CostCenter=01;Users.Name=user01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
+"Name" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Group  Name) is a mandatory field.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Matching Rule" -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Specify the matching rule for creating Dynamic Groups; else leave it empty.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Region" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specify your tenancy's Home Region for creating Groups.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Defined Tags"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
+                              </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
+If the shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::&lt;ocpus&gt;
+"Create_Is PV Encryption In Transit Enabled" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Use this attribute for setting the parameter while launching a new instance. Specify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.Defaults to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">false </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">when left empty.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Update_Is PV Encryption In Transit Enabled"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Use this attribute for setting the parameter for an existing instance. Leave it empty while launching a new instance.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Defined Tags" -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                                 Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
+                               </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Backup Policy" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Leave it empty to not attach any backup policy to the boot volume.
+                                   Values can be either of the following: Gold | Silver | Bronze
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Custom Policy Compartment Name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Specify the name of the compartment where the custom policy is created.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"NSGs"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"DedicatedVMHost"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Leave this field empty if the instance does not need to be launched on dedicated vm host.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Plugin Vulnerability Scanning" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Use this column to enable or disable the 'Vulnerability Scanning' plugin for this instance. Valid values are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enabled or Disabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Enable/Disable 
+other plugins by adding new columns with name as - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Plugin &lt;Plugin_Name_As_It_Appears_In_Console&gt;" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">eg for 'Bastion', column name will be 'Plugin Bastion'
 </t>
     </r>
     <r>
@@ -7898,6 +8284,445 @@
         <i/>
         <u/>
         <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Please add column '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Is Live Migration preferred</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' and set the value to True to enable live migration for the instance. It will be enabled if it is compatible.</t>
+    </r>
+  </si>
+  <si>
+    <t>DB Node Storage Size in GBS</t>
+  </si>
+  <si>
+    <t>Memory Size in GBS</t>
+  </si>
+  <si>
+    <t>Data Storage Size in TBS</t>
+  </si>
+  <si>
+    <t>DB Servers</t>
+  </si>
+  <si>
+    <t>Management Block Volumes</t>
+  </si>
+  <si>
+    <t>Workload Block Volumes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+"SDDC name" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Name of the SDDC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Management Block Volumes" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Existing Block Volume Name (minimum - 8 TB ~ 8192 GB). Format - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip block_compartment if it is same as SDDC comaprtment.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Workload Block Volumes" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Existing Block Volume Names separated by ','. Format - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;,  &lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip block_compartment if it is same as SDDC compartment.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Defined Tags" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
+                             Example: Operations.CostCenter=01;Users.Name=user01</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+** Management and Workload block volumes are needed only if SDDC is of Standard Shape.
+** Standard shapes aren't compatible with Monthly billing interval commitment and advanced HCX license types.</t>
+    </r>
+  </si>
+  <si>
+    <t>Plugin Vulnerability Scanning</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CD3 Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Release - v2024.2.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Allowed values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Network Type" - FLANNEL_OVERLAY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> OCI_VCN_IP_NATIVE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enter subnet name as :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;vcn-name&gt;_&lt;subnet-name&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">or the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ocid
+"API Endpoint Pub Address" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Represents whether public address needs to be assigned to the control plane or not(TRUE|FALSE).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"SSH Key Var Name" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accepts SSH Key value or the name name of the key defined under variable  oke_ssh_keys in variables_&lt;region&gt;.tf filecontaining SSH key; Multiple keys should be separated by \n</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Columns with nsgs accept comma seperated list of NSG names or ocids that needs to be part of the particular component, leave it blank if it doesnot need to be part of any NSG. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
         <color theme="5" tint="-0.249977111117893"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -7976,7 +8801,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Accepts SSH Key value or the name of the variable defined in variables_&lt;region&gt;.tf file containing SSH key; Multiple keys should be separated by \n
+      <t xml:space="preserve"> Accepts SSH Key value or the name of the key defined under variable  instance_ssh_keys in variables_&lt;region&gt;.tf file containing SSH key; Multiple keys should be separated by \n
 </t>
     </r>
     <r>
@@ -8154,831 +8979,6 @@
       </rPr>
       <t xml:space="preserve">
 </t>
-    </r>
-  </si>
-  <si>
-    <t>OCI Networks</t>
-  </si>
-  <si>
-    <t>Public Networks</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
-"Name" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Name) is a mandatory field.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Description" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Description) is a mandatory field.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Public Networks" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">It is an optional field. Specify comma separated list of public CIDRs to be included.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OCI Networks" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">It is an optional field. Format: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Specify comma separated list of VCN CIDR to be included. For ex:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">10.0.2.0/18,10.0.3.0/18
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Defined Tags" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
-                                </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example: Operations.CostCenter=01;Users.Name=user01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
-"Name" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Group  Name) is a mandatory field.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-"Matching Rule" -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Specify the matching rule for creating Dynamic Groups; else leave it empty.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-"Region" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Specify your tenancy's Home Region for creating Groups.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Defined Tags"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
-                              </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Enter subnet name as : &lt;vcn-name&gt;_&lt;subnet-name&gt;
-If the shape is VM.Standard.E3.Flex then specify it as VM.Standard.E3.Flex::&lt;ocpus&gt;
-"Create_Is PV Encryption In Transit Enabled" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Use this attribute for setting the parameter while launching a new instance. Specify </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.Defaults to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">false </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">when left empty.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Update_Is PV Encryption In Transit Enabled"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Use this attribute for setting the parameter for an existing instance. Leave it empty while launching a new instance.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-"Defined Tags" -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                                 Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
-                               </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Example: Operations.CostCenter=01;Users.Name=user01
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Backup Policy" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Leave it empty to not attach any backup policy to the boot volume.
-                                   Values can be either of the following: Gold | Silver | Bronze
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Custom Policy Compartment Name"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Specify the name of the compartment where the custom policy is created.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"NSGs"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Accepts comma seperated list of NSG names instance needs to be part of, leave it blank if instance doesnot need to be part of any NSG.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"DedicatedVMHost"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Leave this field empty if the instance does not need to be launched on dedicated vm host.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Plugin Vulnerability Scanning" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Use this column to enable or disable the 'Vulnerability Scanning' plugin for this instance. Valid values are </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Enabled or Disabled</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Enable/Disable 
-other plugins by adding new columns with name as - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Plugin &lt;Plugin_Name_As_It_Appears_In_Console&gt;" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">eg for 'Bastion', column name will be 'Plugin Bastion'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Please add column '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Is Live Migration preferred</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' and set the value to True to enable live migration for the instance. It will be enabled if it is compatible.</t>
-    </r>
-  </si>
-  <si>
-    <t>DB Node Storage Size in GBS</t>
-  </si>
-  <si>
-    <t>Memory Size in GBS</t>
-  </si>
-  <si>
-    <t>Data Storage Size in TBS</t>
-  </si>
-  <si>
-    <t>DB Servers</t>
-  </si>
-  <si>
-    <t>Management Block Volumes</t>
-  </si>
-  <si>
-    <t>Workload Block Volumes</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-"SDDC name" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Name of the SDDC
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Management Block Volumes" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Existing Block Volume Name (minimum - 8 TB ~ 8192 GB). Format - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Skip block_compartment if it is same as SDDC comaprtment.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Workload Block Volumes" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Existing Block Volume Names separated by ','. Format - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">&lt;block_compartment&gt;@&lt;block-volume_name&gt;,  &lt;block_compartment&gt;@&lt;block-volume_name&gt;. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Skip block_compartment if it is same as SDDC compartment.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Defined Tags" - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
-                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimeter. 
-                             Example: Operations.CostCenter=01;Users.Name=user01</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-** Management and Workload block volumes are needed only if SDDC is of Standard Shape.
-** Standard shapes aren't compatible with Monthly billing interval commitment and advanced HCX license types.</t>
-    </r>
-  </si>
-  <si>
-    <t>Plugin Vulnerability Scanning</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CD3 Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Release - v2024.2.0</t>
     </r>
   </si>
 </sst>
@@ -15061,7 +15061,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -15241,7 +15241,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -15252,7 +15252,7 @@
       <c r="H1" s="85"/>
       <c r="I1" s="86"/>
       <c r="J1" s="91" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="K1" s="91"/>
       <c r="L1" s="91"/>
@@ -15279,7 +15279,7 @@
         <v>216</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>11</v>
@@ -20178,7 +20178,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -20260,7 +20260,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -20337,7 +20337,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -20450,7 +20450,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -20572,7 +20572,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -20591,22 +20591,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>661</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>662</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>663</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>664</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="26" t="s">
         <v>665</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>666</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>269</v>
@@ -20907,7 +20907,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="93" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -20934,22 +20934,22 @@
         <v>216</v>
       </c>
       <c r="E2" s="26" t="s">
+        <v>667</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>668</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G2" s="26" t="s">
         <v>669</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="26" t="s">
         <v>670</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="I2" s="26" t="s">
         <v>671</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>672</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>673</v>
       </c>
       <c r="K2" s="26" t="s">
         <v>269</v>
@@ -21028,7 +21028,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -21093,7 +21093,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -21138,7 +21138,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21168,7 +21168,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="226" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>715</v>
+        <v>729</v>
       </c>
       <c r="B1" s="96"/>
       <c r="C1" s="96"/>
@@ -21178,7 +21178,7 @@
       <c r="G1" s="96"/>
       <c r="H1" s="97"/>
       <c r="I1" s="84" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="J1" s="85"/>
       <c r="K1" s="85"/>
@@ -21239,7 +21239,7 @@
         <v>514</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="P2" s="26" t="s">
         <v>72</v>
@@ -21257,7 +21257,7 @@
         <v>75</v>
       </c>
       <c r="U2" s="27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="V2" s="26" t="s">
         <v>269</v>
@@ -21303,7 +21303,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -21329,7 +21329,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>81</v>
@@ -21404,7 +21404,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="110.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="98" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -21537,7 +21537,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>558</v>
+        <v>728</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -21553,7 +21553,7 @@
       <c r="M1" s="85"/>
       <c r="N1" s="86"/>
       <c r="O1" s="95" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="P1" s="96"/>
       <c r="Q1" s="96"/>
@@ -21706,7 +21706,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -21827,7 +21827,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -22186,7 +22186,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="34" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="88"/>
@@ -22625,7 +22625,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="34" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -22771,7 +22771,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -22905,7 +22905,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -26025,7 +26025,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -28871,7 +28871,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="93" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -28929,16 +28929,16 @@
         <v>490</v>
       </c>
       <c r="K2" s="55" t="s">
+        <v>719</v>
+      </c>
+      <c r="L2" s="55" t="s">
+        <v>720</v>
+      </c>
+      <c r="M2" s="55" t="s">
         <v>721</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="N2" s="55" t="s">
         <v>722</v>
-      </c>
-      <c r="M2" s="55" t="s">
-        <v>723</v>
-      </c>
-      <c r="N2" s="55" t="s">
-        <v>724</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>491</v>
@@ -33204,7 +33204,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="105" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B1" s="106"/>
       <c r="C1" s="106"/>
@@ -33231,43 +33231,43 @@
         <v>6</v>
       </c>
       <c r="C2" s="27" t="s">
+        <v>687</v>
+      </c>
+      <c r="D2" s="64" t="s">
         <v>688</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="E2" s="64" t="s">
         <v>689</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="F2" s="27" t="s">
         <v>690</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="64" t="s">
         <v>691</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="H2" s="27" t="s">
         <v>692</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>693</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>694</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="79" t="s">
+        <v>723</v>
+      </c>
+      <c r="L2" s="80" t="s">
+        <v>724</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>695</v>
       </c>
-      <c r="K2" s="79" t="s">
-        <v>725</v>
-      </c>
-      <c r="L2" s="80" t="s">
-        <v>726</v>
-      </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>696</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="O2" s="27" t="s">
         <v>697</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>698</v>
       </c>
       <c r="P2" s="27" t="s">
         <v>72</v>
@@ -33320,7 +33320,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B1" s="96"/>
       <c r="C1" s="96"/>
@@ -33341,43 +33341,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C2" s="64" t="s">
+        <v>699</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>700</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="27" t="s">
         <v>701</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="27" t="s">
         <v>702</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>703</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="27" t="s">
         <v>704</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="27" t="s">
         <v>705</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="J2" s="27" t="s">
         <v>706</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="27" t="s">
         <v>707</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="L2" s="27" t="s">
         <v>708</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>709</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="N2" s="27" t="s">
         <v>710</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>711</v>
       </c>
       <c r="O2" s="41"/>
     </row>
@@ -33390,7 +33390,7 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -33436,7 +33436,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="261" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="108" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B1" s="109"/>
       <c r="C1" s="109"/>
@@ -33464,49 +33464,49 @@
         <v>6</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>629</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>630</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="26" t="s">
         <v>631</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="26" t="s">
+        <v>643</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>642</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>634</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>641</v>
+      </c>
+      <c r="J2" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>644</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>643</v>
-      </c>
-      <c r="H2" s="26" t="s">
+      <c r="K2" s="27" t="s">
+        <v>633</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>640</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>639</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>638</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>637</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>636</v>
+      </c>
+      <c r="Q2" s="27" t="s">
         <v>635</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>642</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>633</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>634</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>641</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>640</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>639</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>638</v>
-      </c>
-      <c r="P2" s="27" t="s">
-        <v>637</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>636</v>
       </c>
       <c r="R2" s="26" t="s">
         <v>269</v>
@@ -33718,10 +33718,10 @@
         <v>539</v>
       </c>
       <c r="AM1" s="45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AN1" s="45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:40" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -33729,22 +33729,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F2" s="48" t="s">
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H2" s="48" t="s">
         <v>28</v>
@@ -33756,13 +33756,13 @@
         <v>43</v>
       </c>
       <c r="K2" s="48" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="L2" s="48" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="48" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="N2" s="48" t="s">
         <v>393</v>
@@ -33783,10 +33783,10 @@
         <v>251</v>
       </c>
       <c r="T2" s="48" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="U2" s="48" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="V2" s="48" t="s">
         <v>431</v>
@@ -33837,13 +33837,13 @@
         <v>221</v>
       </c>
       <c r="AL2" s="47" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AM2" s="47" t="b">
         <v>0</v>
       </c>
       <c r="AN2" s="47" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:40" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -33851,16 +33851,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F3" s="48" t="s">
         <v>20</v>
@@ -33901,7 +33901,7 @@
         <v>434</v>
       </c>
       <c r="T3" s="48" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="U3" s="48"/>
       <c r="V3" s="48" t="s">
@@ -33953,13 +33953,13 @@
         <v>222</v>
       </c>
       <c r="AL3" s="47" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AM3" s="47" t="b">
         <v>1</v>
       </c>
       <c r="AN3" s="47" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:40" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -33967,16 +33967,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F4" s="48"/>
       <c r="G4" t="s">
@@ -34007,7 +34007,7 @@
         <v>438</v>
       </c>
       <c r="T4" s="48" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="U4" s="48"/>
       <c r="V4" s="48"/>
@@ -34045,7 +34045,7 @@
         <v>32</v>
       </c>
       <c r="AN4" s="47" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:40" s="47" customFormat="1" x14ac:dyDescent="0.2">
@@ -34053,14 +34053,14 @@
         <v>6</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F5" s="48"/>
       <c r="G5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H5" s="48"/>
       <c r="I5" s="48" t="s">
@@ -34110,14 +34110,14 @@
         <v>7</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F6" s="48"/>
       <c r="G6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H6" s="48"/>
       <c r="I6" s="48"/>
@@ -34159,10 +34159,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F7" s="48"/>
       <c r="G7" t="s">
@@ -34206,10 +34206,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" t="s">
@@ -34253,10 +34253,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" t="s">
@@ -34300,14 +34300,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F10" s="48"/>
       <c r="G10" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
@@ -34347,14 +34347,14 @@
         <v>12</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F11" s="48"/>
       <c r="G11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
@@ -34395,7 +34395,7 @@
       </c>
       <c r="F12" s="48"/>
       <c r="G12" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H12" s="48"/>
       <c r="I12" s="48"/>
@@ -34434,7 +34434,7 @@
       </c>
       <c r="F13" s="48"/>
       <c r="G13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H13" s="48"/>
       <c r="I13" s="48"/>
@@ -34473,7 +34473,7 @@
       </c>
       <c r="F14" s="48"/>
       <c r="G14" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H14" s="48"/>
       <c r="I14" s="48"/>
@@ -34590,7 +34590,7 @@
       </c>
       <c r="F17" s="48"/>
       <c r="G17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H17" s="48"/>
       <c r="I17" s="48"/>
@@ -34629,7 +34629,7 @@
       </c>
       <c r="F18" s="48"/>
       <c r="G18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H18" s="48"/>
       <c r="I18" s="48"/>
@@ -34668,7 +34668,7 @@
       </c>
       <c r="F19" s="48"/>
       <c r="G19" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H19" s="48"/>
       <c r="I19" s="48"/>
@@ -34707,7 +34707,7 @@
       </c>
       <c r="F20" s="48"/>
       <c r="G20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H20" s="48"/>
       <c r="I20" s="48"/>
@@ -34785,7 +34785,7 @@
       </c>
       <c r="F22" s="48"/>
       <c r="G22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H22" s="48"/>
       <c r="I22" s="48"/>
@@ -34824,7 +34824,7 @@
       </c>
       <c r="F23" s="48"/>
       <c r="G23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H23" s="48"/>
       <c r="I23" s="48"/>
@@ -34863,7 +34863,7 @@
       </c>
       <c r="F24" s="48"/>
       <c r="G24" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H24" s="48"/>
       <c r="I24" s="48"/>
@@ -34941,7 +34941,7 @@
       </c>
       <c r="F26" s="48"/>
       <c r="G26" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H26" s="48"/>
       <c r="I26" s="48"/>
@@ -35058,7 +35058,7 @@
       </c>
       <c r="F29" s="48"/>
       <c r="G29" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H29" s="48"/>
       <c r="I29" s="48"/>
@@ -35136,7 +35136,7 @@
       </c>
       <c r="F31" s="48"/>
       <c r="G31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H31" s="48"/>
       <c r="I31" s="48"/>
@@ -35214,7 +35214,7 @@
       </c>
       <c r="F33" s="48"/>
       <c r="G33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H33" s="48"/>
       <c r="I33" s="48"/>
@@ -35253,7 +35253,7 @@
       </c>
       <c r="F34" s="48"/>
       <c r="G34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H34" s="48"/>
       <c r="I34" s="48"/>
@@ -35331,7 +35331,7 @@
       </c>
       <c r="F36" s="48"/>
       <c r="G36" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H36" s="48"/>
       <c r="I36" s="48"/>
@@ -35409,7 +35409,7 @@
       </c>
       <c r="F38" s="48"/>
       <c r="G38" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H38" s="48"/>
       <c r="I38" s="48"/>
@@ -35448,7 +35448,7 @@
       </c>
       <c r="F39" s="48"/>
       <c r="G39" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H39" s="48"/>
       <c r="I39" s="48"/>
@@ -35917,7 +35917,7 @@
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F12" s="29"/>
       <c r="H12" s="29" t="s">
@@ -35934,7 +35934,7 @@
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F13" s="29"/>
       <c r="H13" s="29" t="s">
@@ -36455,7 +36455,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="34" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -36469,19 +36469,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="26" t="s">
+        <v>624</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>625</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>628</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>629</v>
       </c>
       <c r="G2" s="26" t="s">
         <v>269</v>
@@ -37525,7 +37525,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -37533,7 +37533,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -37541,7 +37541,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -37549,7 +37549,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -37846,7 +37846,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="34" customFormat="1" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="82"/>
@@ -37865,10 +37865,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>269</v>
@@ -39447,7 +39447,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="34" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="81" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -41803,7 +41803,7 @@
       <c r="E1" s="85"/>
       <c r="F1" s="86"/>
       <c r="G1" s="87" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H1" s="88"/>
       <c r="I1" s="89"/>
@@ -41877,7 +41877,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="187.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -41885,7 +41885,7 @@
       <c r="E1" s="85"/>
       <c r="F1" s="86"/>
       <c r="G1" s="84" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H1" s="85"/>
       <c r="I1" s="85"/>
@@ -41979,7 +41979,7 @@
       <c r="E1" s="81"/>
       <c r="F1" s="81"/>
       <c r="G1" s="90" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H1" s="90"/>
       <c r="I1" s="90"/>
@@ -41998,7 +41998,7 @@
         <v>396</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.3.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19569292-BC0A-B14D-B0E7-0CBCFE65E647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE011F5-6BF6-964D-BE2C-54919FBFB3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6940" yWindow="760" windowWidth="30240" windowHeight="17420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Mansatory for Autotune Type - PERFORMANCE_BASED or BOTH</t>
+          <t>Mandatory for Autotune Type - PERFORMANCE_BASED or BOTH</t>
         </r>
       </text>
     </comment>
@@ -382,30 +382,6 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Suruchi</author>
-  </authors>
-  <commentList>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{DFA3381A-B6E3-8642-9D9B-F59DB2F382DA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mansatory for Autotune Type - PERFORMANCE_BASED or BOTH</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
@@ -650,7 +626,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Suruchi</author>
@@ -712,7 +688,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="775">
   <si>
     <t>Region</t>
   </si>
@@ -10327,12 +10303,318 @@
   <si>
     <t>Matching Rule</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Default value for columns if left blank: sourceCIDR- 0.0.0.0/0, Access- READ_WRITE, GID- 65534, UID- 65534, IDSquash- NONE and Require PS Port- false.
+Mount target IP will take default values from OCI if left blank.
+Resources will be created based on 'MountTarget Name' and 'FSS Name' columns.
+Below sample data shows example of  multiple FSS(FSS1 and FSS2) using single MT(MT1) , 1 FSS(FSS3) using multiple MTs(MT2 and MT3) and also 1 FSS(FSS4) using 1 MT(MT4).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>onlyMT is Mount target without any FSS. onlyFSS is File System without any Mount Target or Export (used for replication)</t>
+    </r>
+  </si>
+  <si>
+    <t>MountTarget Name</t>
+  </si>
+  <si>
+    <t>MountTarget SubnetName</t>
+  </si>
+  <si>
+    <t>MountTarget IP</t>
+  </si>
+  <si>
+    <t>MountTarget Hostname</t>
+  </si>
+  <si>
+    <t>FSS Name</t>
+  </si>
+  <si>
+    <t>Source Snapshot</t>
+  </si>
+  <si>
+    <t>Snapshot Policy</t>
+  </si>
+  <si>
+    <t>Replication Information</t>
+  </si>
+  <si>
+    <t>Source CIDR</t>
+  </si>
+  <si>
+    <t>Access (READ_ONLY|READ_WRITE)</t>
+  </si>
+  <si>
+    <t>GID</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>IDSquash (NONE|ALL|ROOT)</t>
+  </si>
+  <si>
+    <t>Require PS Port (true|false)</t>
+  </si>
+  <si>
+    <t>Is Anonymous Access Allowed</t>
+  </si>
+  <si>
+    <t>Allowed Auth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+Columns: Region, Compartment Name, Availability Domain, MountTarget Name, MountTarget SubnetName, FSS name, Path are mandatory.
+Freeform and Defined Tags - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If specified, Applies to FSS object only and not to other components like Mount Target.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Enter subnet name as : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">vcn-name&gt;_&lt;subnet-name&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source Snapshot:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Accepts OCID of the source snapshot  or the name of the key defined under variable  fss_source_ocids in variables_&lt;region&gt;.tf file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Snapshot Policy - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accepts OCID of the snapshot policy or the name in format: &lt;snaphot_policy_compartment_name&gt;@&lt;snaphost_policy_name&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Replication Information: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Format - TargetFSS(OCID or Name)::ReplicationInterval::ReplicationName. Multiple replication values are seperated by newline in the same cell(\n is not supported). Ensure Target FSS for replication must not have exports created.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+"Defined Tags" - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Specify the defined tag key and its value in the format - &lt;Namespace&gt;.&lt;TagKey&gt;=&lt;Value&gt;  else leave it empty.
+                             Multiple Tag Key , Values can be specified using semi colon (;) as the delimiter. 
+                           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Example: Operations.CostCenter=01;Users.Name=user01</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10658,6 +10940,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -10924,7 +11215,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11203,6 +11494,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -22837,7 +23137,7 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
@@ -22951,14 +23251,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView zoomScale="89" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22972,8 +23272,8 @@
     <col min="8" max="8" width="8.5" customWidth="1"/>
     <col min="9" max="9" width="9.83203125" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="8.5" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" customWidth="1"/>
     <col min="15" max="15" width="15.5" customWidth="1"/>
@@ -22981,9 +23281,9 @@
     <col min="17" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="201" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="97" t="s">
-        <v>749</v>
+        <v>774</v>
       </c>
       <c r="B1" s="98"/>
       <c r="C1" s="98"/>
@@ -22995,84 +23295,99 @@
       <c r="I1" s="98"/>
       <c r="J1" s="98"/>
       <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="101"/>
-    </row>
-    <row r="2" spans="1:18" s="33" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="L1" s="101"/>
+      <c r="M1" s="113" t="s">
+        <v>757</v>
+      </c>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="115"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>655</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>81</v>
+      <c r="C2" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>758</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>759</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>66</v>
+        <v>760</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>82</v>
+        <v>761</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I2" s="26" t="s">
-        <v>503</v>
+        <v>762</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>262</v>
+        <v>763</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>725</v>
+        <v>764</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>726</v>
+        <v>765</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>727</v>
+        <v>85</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>728</v>
+        <v>766</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>502</v>
+        <v>767</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>73</v>
+        <v>768</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>377</v>
+        <v>769</v>
       </c>
       <c r="R2" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>771</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>772</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>773</v>
+      </c>
+      <c r="V2" s="26" t="s">
         <v>258</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="M1:V1"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation allowBlank="1" sqref="A3:XFD1048576 A1:J2 L1:M2 O1:XFD2 N1" xr:uid="{02462EBB-6C3D-AD4C-90E1-0F01761ACD92}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{44F44AA6-F9A2-F043-9A7C-E9C593C12245}"/>
-    <dataValidation type="list" sqref="K1:K2" xr:uid="{296BAB61-C7D2-7746-8608-28C808FD0978}">
-      <formula1>"BOTH,PERFORMANCE_BASED,DETACHED_VOLUME"</formula1>
-    </dataValidation>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" sqref="A3:XFD1048576 U1:XFD2 B2:L2 M1:S2 A1:A2" xr:uid="{02462EBB-6C3D-AD4C-90E1-0F01761ACD92}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="T1:T2" xr:uid="{7A2F3F2A-4835-1545-9D47-36E98CCE349F}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -23695,15 +24010,15 @@
       <c r="J1" s="102" t="s">
         <v>267</v>
       </c>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="114"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="116"/>
+      <c r="N1" s="116"/>
+      <c r="O1" s="116"/>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="117"/>
     </row>
     <row r="2" spans="1:19" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -31388,26 +31703,26 @@
       <c r="A1" s="108" t="s">
         <v>663</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
       <c r="V1" s="60"/>
       <c r="W1" s="60"/>
       <c r="X1" s="60"/>
@@ -35718,26 +36033,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="119" t="s">
         <v>710</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="121"/>
     </row>
     <row r="2" spans="1:18" s="40" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -35967,26 +36282,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="261" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="122" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="121"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="124"/>
     </row>
     <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.4.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/CD3Lasya/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62626BD-3037-C149-AE13-3DED4F39E581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0C9CFB-37FE-B544-BFED-C52E67530D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="760" windowWidth="29840" windowHeight="17420" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38401,9 +38401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1F6A15-066C-494D-992B-F6A4A794D67F}">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Automation Toolkit Release v2024.4.3
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067F5F34-0EB6-C04E-AFDD-C47520B25E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96238EC-EEFD-6441-9101-2FBA2FAA7E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1100" windowWidth="26580" windowHeight="17300" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8560" yWindow="1140" windowWidth="26580" windowHeight="17300" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <definedName name="workload_drop" localSheetId="3">#REF!</definedName>
     <definedName name="workload_drop">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5810,493 +5810,6 @@
     <t>Domain Name</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Vault Display Name(mandatory)"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Should Not be more than 100 characters and should contain only Alpha-Numeric Characters, underscores, hyphens.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Vault Type(mandatory)"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Valid values are</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"virtual_private</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Replica Region(optional)"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Valid only for vault type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"virtual_private"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Can't be same as the primary vault region.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Key details can be left empty if no keys have to be created in the specified vault.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If a key/keys have to be created, enter below </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>mandatory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> fields:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Key Compartment Name" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-  can be same as the Vault compartment or a different compartment.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Key Display Name"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Should Not be more than 100 characters and should contain only Alpha-Numeric Characters, underscores, hyphens
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Protection Mode" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Valid values are </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"HSM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" or </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"SOFTWARE".</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Algorithm" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Valid values are </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"AES", "RSA", "ECDSA". </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Length in bits" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Valid values for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"AES"  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      -  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>128, 192, 256</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                                                                           </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"RSA" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2048, 3072, 4096</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                                                                          "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ECDSA"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   -  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>256, 384, 521</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>Vault Compartment Name</t>
   </si>
   <si>
@@ -10448,51 +9961,6 @@
       <t xml:space="preserve">
 ** Management and Workload block volumes are needed only if SDDC is of Standard Shape.
 ** Standard shapes aren't compatible with Monthly billing interval commitment and advanced HCX license types.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CD3 Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Release - v2024.4.2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
- Modified description for VCNs, DRGs, BlockVolumes, SDDCs Tabs. Added a note in Exa-VMClusters Tab.</t>
     </r>
   </si>
   <si>
@@ -10773,6 +10241,559 @@
       </rPr>
       <t xml:space="preserve">
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Vault Display Name(mandatory)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Should Not be more than 100 characters and should contain only Alpha-Numeric Characters, underscores, hyphens.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Vault Type(mandatory)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Valid values are</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"virtual_private</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Replica Region(optional)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Valid for both </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"virtual_private"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" vault types. Can't be same as the primary vault region.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Key details can be left empty if no keys have to be created in the specified vault.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If a key/keys have to be created, enter below </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mandatory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fields:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Key Compartment Name" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-  can be same as the Vault compartment or a different compartment.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Key Display Name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Should Not be more than 100 characters and should contain only Alpha-Numeric Characters, underscores, hyphens
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Protection Mode" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Valid values are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"HSM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"SOFTWARE".</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Algorithm" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Valid values are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"AES", "RSA", "ECDSA". </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Length in bits" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Valid values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"AES"  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      -  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>128, 192, 256</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"RSA" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2048, 3072, 4096</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                                                                          "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ECDSA"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   -  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>256, 384, 521</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CD3 Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Release - v2024.4.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ Modified description in KMS sheet, Modified delimiters in ServiceConectors sheet</t>
     </r>
   </si>
 </sst>
@@ -16913,7 +16934,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
     </row>
   </sheetData>
@@ -16957,7 +16978,7 @@
       <c r="E1" s="100"/>
       <c r="F1" s="101"/>
       <c r="G1" s="99" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="H1" s="100"/>
       <c r="I1" s="100"/>
@@ -17043,7 +17064,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -17118,7 +17139,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B1" s="104"/>
     </row>
@@ -17185,7 +17206,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -23196,7 +23217,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="226" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
@@ -23206,7 +23227,7 @@
       <c r="G1" s="111"/>
       <c r="H1" s="112"/>
       <c r="I1" s="99" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J1" s="100"/>
       <c r="K1" s="100"/>
@@ -23239,7 +23260,7 @@
         <v>67</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>69</v>
@@ -23330,7 +23351,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="201" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -23456,7 +23477,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -23470,7 +23491,7 @@
       <c r="K1" s="100"/>
       <c r="L1" s="101"/>
       <c r="M1" s="113" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="N1" s="114"/>
       <c r="O1" s="114"/>
@@ -23493,58 +23514,58 @@
         <v>65</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>739</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>719</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>740</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>720</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>721</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>73</v>
       </c>
       <c r="I2" s="25" t="s">
+        <v>721</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>724</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>725</v>
       </c>
       <c r="M2" s="25" t="s">
         <v>84</v>
       </c>
       <c r="N2" s="25" t="s">
+        <v>725</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>726</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="25" t="s">
         <v>727</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>728</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="R2" s="25" t="s">
         <v>729</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="S2" s="25" t="s">
         <v>730</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="T2" s="25" t="s">
         <v>731</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="U2" s="25" t="s">
         <v>732</v>
-      </c>
-      <c r="U2" s="25" t="s">
-        <v>733</v>
       </c>
       <c r="V2" s="25" t="s">
         <v>255</v>
@@ -23615,7 +23636,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -23632,7 +23653,7 @@
       <c r="N1" s="100"/>
       <c r="O1" s="101"/>
       <c r="P1" s="110" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="Q1" s="111"/>
       <c r="R1" s="111"/>
@@ -23677,10 +23698,10 @@
         <v>517</v>
       </c>
       <c r="H2" s="25" t="s">
+        <v>742</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>743</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>744</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>518</v>
@@ -23695,7 +23716,7 @@
         <v>521</v>
       </c>
       <c r="N2" s="25" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="O2" s="25" t="s">
         <v>522</v>
@@ -23719,7 +23740,7 @@
         <v>524</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="W2" s="25" t="s">
         <v>65</v>
@@ -23734,7 +23755,7 @@
         <v>526</v>
       </c>
       <c r="AA2" s="25" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="AB2" s="25" t="s">
         <v>527</v>
@@ -23805,7 +23826,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -23846,7 +23867,7 @@
         <v>386</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>88</v>
@@ -23926,7 +23947,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -23970,7 +23991,7 @@
         <v>97</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>98</v>
@@ -24056,7 +24077,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -24288,7 +24309,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="30" customFormat="1" ht="173" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="96" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -24311,10 +24332,10 @@
         <v>701</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>255</v>
@@ -25107,7 +25128,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="106" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -25121,7 +25142,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>636</v>
@@ -25196,7 +25217,7 @@
         <v>500</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>501</v>
@@ -25599,7 +25620,7 @@
         <v>266</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -25640,7 +25661,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -25669,7 +25690,7 @@
         <v>507</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>508</v>
@@ -25774,7 +25795,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="100"/>
@@ -25814,7 +25835,7 @@
         <v>65</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>448</v>
@@ -31740,7 +31761,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
@@ -31780,10 +31801,10 @@
         <v>471</v>
       </c>
       <c r="E2" s="38" t="s">
+        <v>755</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>756</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>757</v>
       </c>
       <c r="G2" s="38" t="s">
         <v>450</v>
@@ -36075,7 +36096,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="118" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -36208,7 +36229,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
@@ -36232,7 +36253,7 @@
         <v>643</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>654</v>
@@ -36313,7 +36334,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="30" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -36331,16 +36352,16 @@
         <v>596</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>763</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>764</v>
       </c>
       <c r="G2" s="93" t="s">
         <v>701</v>
@@ -37441,7 +37462,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>702</v>
+        <v>772</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -37450,7 +37471,7 @@
       <c r="F1" s="95"/>
       <c r="G1" s="95"/>
       <c r="H1" s="102" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I1" s="116"/>
       <c r="J1" s="116"/>
@@ -37465,46 +37486,46 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2" s="85" t="s">
         <v>703</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="D2" s="15" t="s">
         <v>704</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>705</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>707</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>708</v>
+      </c>
+      <c r="H2" s="60" t="s">
+        <v>709</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="J2" s="86" t="s">
+        <v>711</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>713</v>
+      </c>
+      <c r="M2" s="87" t="s">
+        <v>714</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>706</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>708</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>709</v>
-      </c>
-      <c r="H2" s="60" t="s">
-        <v>710</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="J2" s="86" t="s">
-        <v>712</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>713</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>714</v>
-      </c>
-      <c r="M2" s="87" t="s">
+      <c r="O2" s="15" t="s">
         <v>715</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>707</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -42156,7 +42177,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="30" customFormat="1" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>
@@ -43757,7 +43778,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="30" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B1" s="95"/>
       <c r="C1" s="95"/>
@@ -46252,7 +46273,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="30" customFormat="1" ht="207" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="95" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B1" s="97"/>
       <c r="C1" s="97"/>

</xml_diff>

<commit_message>
Automation Toolkit Release v2025.1.0
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96238EC-EEFD-6441-9101-2FBA2FAA7E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B09B020-5AB5-164E-9D43-55CFE6631EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8560" yWindow="1140" windowWidth="26580" windowHeight="17300" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="860" windowWidth="26580" windowHeight="17300" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -36177,9 +36177,7 @@
     <mergeCell ref="A1:R1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" sqref="H3:H1048576" xr:uid="{89BA7024-AC40-C54B-96AA-4FB1476BE9A7}">
-      <formula1>"AD1,AD2,AD3,multi-AD"</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" sqref="H3:H1048576" xr:uid="{89BA7024-AC40-C54B-96AA-4FB1476BE9A7}"/>
     <dataValidation type="list" allowBlank="1" sqref="G3:G1048576" xr:uid="{A0359C5C-7BD6-EA4B-8F45-D40E7142A750}">
       <formula1>"HOUR,MONTH,ONE_YEAR,THREE_YEARS"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Automation Toolkit Release v2025.1.2
</commit_message>
<xml_diff>
--- a/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
+++ b/cd3_automation_toolkit/example/CD3-Blank-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lasyavadavalli/PycharmProjects/CD3Lasya/cd3_automation_toolkit/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susingla/PyCharmProjects/orahub-develop/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263BE640-A49C-C143-9D56-2DE14628165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390AFC42-23F2-2648-8A88-88D76E536C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,7 +835,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="799">
   <si>
     <t>Region</t>
   </si>
@@ -3331,9 +3331,6 @@
     <t>Saopaulo</t>
   </si>
   <si>
-    <t>Singapore</t>
-  </si>
-  <si>
     <t>Stockholm</t>
   </si>
   <si>
@@ -11364,6 +11361,12 @@
   </si>
   <si>
     <t>users_variable_value</t>
+  </si>
+  <si>
+    <t>Singapore-1</t>
+  </si>
+  <si>
+    <t>Singapore-2</t>
   </si>
 </sst>
 </file>
@@ -17532,7 +17535,7 @@
     <row r="1" spans="1:1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -17572,7 +17575,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="247" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -17580,7 +17583,7 @@
       <c r="E1" s="104"/>
       <c r="F1" s="105"/>
       <c r="G1" s="103" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H1" s="104"/>
       <c r="I1" s="104"/>
@@ -17670,7 +17673,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -17678,7 +17681,7 @@
       <c r="E1" s="99"/>
       <c r="F1" s="99"/>
       <c r="G1" s="109" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H1" s="109"/>
       <c r="I1" s="109"/>
@@ -17697,7 +17700,7 @@
         <v>379</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>380</v>
@@ -17749,7 +17752,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="30" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B1" s="108"/>
     </row>
@@ -17820,7 +17823,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -17908,7 +17911,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -17919,7 +17922,7 @@
       <c r="H1" s="104"/>
       <c r="I1" s="105"/>
       <c r="J1" s="110" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K1" s="110"/>
       <c r="L1" s="110"/>
@@ -17946,7 +17949,7 @@
         <v>203</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>11</v>
@@ -22849,7 +22852,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -22935,7 +22938,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -23016,7 +23019,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -23133,7 +23136,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -23259,7 +23262,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>
@@ -23278,22 +23281,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>624</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>625</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>626</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>627</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>628</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>629</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>255</v>
@@ -23593,7 +23596,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="30" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -23661,7 +23664,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="208" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="112" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B1" s="113"/>
       <c r="C1" s="113"/>
@@ -23688,22 +23691,22 @@
         <v>203</v>
       </c>
       <c r="E2" s="24" t="s">
+        <v>630</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>631</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>632</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>634</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>635</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>636</v>
       </c>
       <c r="K2" s="24" t="s">
         <v>255</v>
@@ -23786,7 +23789,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -23871,7 +23874,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="226" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="114" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B1" s="115"/>
       <c r="C1" s="115"/>
@@ -23881,7 +23884,7 @@
       <c r="G1" s="115"/>
       <c r="H1" s="116"/>
       <c r="I1" s="103" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J1" s="104"/>
       <c r="K1" s="104"/>
@@ -23914,7 +23917,7 @@
         <v>67</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>69</v>
@@ -23941,7 +23944,7 @@
         <v>494</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>71</v>
@@ -23959,7 +23962,7 @@
         <v>74</v>
       </c>
       <c r="U2" s="25" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="V2" s="24" t="s">
         <v>255</v>
@@ -24009,7 +24012,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="201" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -24040,7 +24043,7 @@
         <v>79</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>80</v>
@@ -24061,16 +24064,16 @@
         <v>258</v>
       </c>
       <c r="K2" s="25" t="s">
+        <v>695</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>696</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>697</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>698</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>699</v>
       </c>
       <c r="O2" s="25" t="s">
         <v>495</v>
@@ -24139,7 +24142,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="169" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -24153,7 +24156,7 @@
       <c r="K1" s="104"/>
       <c r="L1" s="105"/>
       <c r="M1" s="117" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="N1" s="118"/>
       <c r="O1" s="118"/>
@@ -24176,58 +24179,58 @@
         <v>65</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>738</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>718</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>739</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>719</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>720</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>73</v>
       </c>
       <c r="I2" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>722</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>723</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>724</v>
       </c>
       <c r="M2" s="25" t="s">
         <v>84</v>
       </c>
       <c r="N2" s="25" t="s">
+        <v>724</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="25" t="s">
         <v>726</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>727</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="R2" s="25" t="s">
         <v>728</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="S2" s="25" t="s">
         <v>729</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="T2" s="25" t="s">
         <v>730</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="U2" s="25" t="s">
         <v>731</v>
-      </c>
-      <c r="U2" s="25" t="s">
-        <v>732</v>
       </c>
       <c r="V2" s="25" t="s">
         <v>255</v>
@@ -24302,7 +24305,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -24319,7 +24322,7 @@
       <c r="N1" s="104"/>
       <c r="O1" s="105"/>
       <c r="P1" s="114" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="Q1" s="115"/>
       <c r="R1" s="115"/>
@@ -24352,7 +24355,7 @@
         <v>514</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>515</v>
@@ -24364,10 +24367,10 @@
         <v>517</v>
       </c>
       <c r="H2" s="25" t="s">
+        <v>741</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>742</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>743</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>518</v>
@@ -24382,7 +24385,7 @@
         <v>521</v>
       </c>
       <c r="N2" s="25" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="O2" s="25" t="s">
         <v>522</v>
@@ -24406,13 +24409,13 @@
         <v>524</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W2" s="25" t="s">
         <v>65</v>
       </c>
       <c r="X2" s="25" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Y2" s="25" t="s">
         <v>525</v>
@@ -24421,7 +24424,7 @@
         <v>526</v>
       </c>
       <c r="AA2" s="25" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AB2" s="25" t="s">
         <v>527</v>
@@ -24439,13 +24442,13 @@
         <v>529</v>
       </c>
       <c r="AG2" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="AH2" s="25" t="s">
         <v>679</v>
       </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AI2" s="25" t="s">
         <v>680</v>
-      </c>
-      <c r="AI2" s="25" t="s">
-        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -24496,7 +24499,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="122.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -24537,7 +24540,7 @@
         <v>386</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>88</v>
@@ -24621,7 +24624,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -24665,7 +24668,7 @@
         <v>97</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>98</v>
@@ -24755,7 +24758,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -24995,7 +24998,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="30" customFormat="1" ht="173" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="100" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -25015,13 +25018,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E2" s="91" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F2" s="72" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G2" s="72" t="s">
         <v>255</v>
@@ -25761,7 +25764,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="30" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B1" s="107"/>
       <c r="C1" s="107"/>
@@ -25822,7 +25825,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -25836,10 +25839,10 @@
         <v>87</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25915,7 +25918,7 @@
         <v>500</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>501</v>
@@ -26307,10 +26310,10 @@
         <v>505</v>
       </c>
       <c r="G2" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>700</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>701</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>100</v>
@@ -26322,7 +26325,7 @@
         <v>266</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
   </sheetData>
@@ -26367,7 +26370,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -26396,7 +26399,7 @@
         <v>507</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>508</v>
@@ -26505,7 +26508,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -26545,7 +26548,7 @@
         <v>65</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>448</v>
@@ -29629,7 +29632,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="103" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -32479,7 +32482,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="114" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B1" s="115"/>
       <c r="C1" s="115"/>
@@ -32519,10 +32522,10 @@
         <v>471</v>
       </c>
       <c r="E2" s="38" t="s">
+        <v>754</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>755</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>756</v>
       </c>
       <c r="G2" s="38" t="s">
         <v>450</v>
@@ -32537,16 +32540,16 @@
         <v>472</v>
       </c>
       <c r="K2" s="94" t="s">
+        <v>669</v>
+      </c>
+      <c r="L2" s="94" t="s">
         <v>670</v>
       </c>
-      <c r="L2" s="94" t="s">
+      <c r="M2" s="38" t="s">
         <v>671</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="N2" s="38" t="s">
         <v>672</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>673</v>
       </c>
       <c r="O2" s="38" t="s">
         <v>473</v>
@@ -36818,7 +36821,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="122" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -36846,46 +36849,46 @@
         <v>6</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>642</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>681</v>
+      </c>
+      <c r="E2" s="56" t="s">
         <v>643</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>682</v>
-      </c>
-      <c r="E2" s="56" t="s">
+      <c r="F2" s="56" t="s">
         <v>644</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="G2" s="25" t="s">
         <v>645</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="56" t="s">
         <v>646</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="I2" s="25" t="s">
         <v>647</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>648</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>649</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="71" t="s">
+        <v>673</v>
+      </c>
+      <c r="M2" s="71" t="s">
+        <v>674</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>650</v>
       </c>
-      <c r="L2" s="71" t="s">
-        <v>674</v>
-      </c>
-      <c r="M2" s="71" t="s">
-        <v>675</v>
-      </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="P2" s="25" t="s">
         <v>652</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>653</v>
       </c>
       <c r="Q2" s="25" t="s">
         <v>71</v>
@@ -36953,7 +36956,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="114" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -36974,43 +36977,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>653</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>654</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>655</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>656</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>657</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>658</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>659</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>660</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" s="25" t="s">
         <v>661</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>662</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>663</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>664</v>
       </c>
       <c r="O2" s="37"/>
     </row>
@@ -37023,7 +37026,7 @@
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -37062,7 +37065,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="30" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -37077,22 +37080,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>762</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>763</v>
-      </c>
       <c r="G2" s="93" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>255</v>
@@ -38044,7 +38047,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="270" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="125" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B1" s="126"/>
       <c r="C1" s="126"/>
@@ -38072,49 +38075,49 @@
         <v>6</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>597</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
         <v>598</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
+        <v>610</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>609</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>608</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>611</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>610</v>
-      </c>
-      <c r="H2" s="24" t="s">
+      <c r="K2" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>606</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>605</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q2" s="25" t="s">
         <v>602</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>609</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>600</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>601</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>608</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>607</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>606</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>605</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>604</v>
-      </c>
-      <c r="Q2" s="25" t="s">
-        <v>603</v>
       </c>
       <c r="R2" s="24" t="s">
         <v>255</v>
@@ -38198,7 +38201,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -38207,7 +38210,7 @@
       <c r="F1" s="99"/>
       <c r="G1" s="99"/>
       <c r="H1" s="106" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I1" s="120"/>
       <c r="J1" s="120"/>
@@ -38222,46 +38225,46 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2" s="85" t="s">
         <v>702</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="D2" s="15" t="s">
         <v>703</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>704</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>706</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>707</v>
+      </c>
+      <c r="H2" s="60" t="s">
+        <v>708</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>709</v>
+      </c>
+      <c r="J2" s="86" t="s">
+        <v>710</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>711</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="M2" s="87" t="s">
+        <v>713</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>705</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>707</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>708</v>
-      </c>
-      <c r="H2" s="60" t="s">
-        <v>709</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>710</v>
-      </c>
-      <c r="J2" s="86" t="s">
-        <v>711</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>712</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>713</v>
-      </c>
-      <c r="M2" s="87" t="s">
+      <c r="O2" s="15" t="s">
         <v>714</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>706</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -39407,7 +39410,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="212" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="128" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -39417,7 +39420,7 @@
       <c r="G1" s="123"/>
       <c r="H1" s="124"/>
       <c r="I1" s="114" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J1" s="115"/>
       <c r="K1" s="115"/>
@@ -39454,10 +39457,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="96" t="s">
+        <v>775</v>
+      </c>
+      <c r="F2" s="95" t="s">
         <v>776</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>777</v>
       </c>
       <c r="G2" s="96" t="s">
         <v>65</v>
@@ -39466,64 +39469,64 @@
         <v>67</v>
       </c>
       <c r="I2" s="96" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J2" s="95" t="s">
         <v>66</v>
       </c>
       <c r="K2" s="95" t="s">
+        <v>777</v>
+      </c>
+      <c r="L2" s="95" t="s">
         <v>778</v>
-      </c>
-      <c r="L2" s="95" t="s">
-        <v>779</v>
       </c>
       <c r="M2" s="96" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="96" t="s">
+        <v>779</v>
+      </c>
+      <c r="O2" s="96" t="s">
         <v>780</v>
       </c>
-      <c r="O2" s="96" t="s">
+      <c r="P2" s="96" t="s">
         <v>781</v>
       </c>
-      <c r="P2" s="96" t="s">
+      <c r="Q2" s="96" t="s">
         <v>782</v>
       </c>
-      <c r="Q2" s="96" t="s">
+      <c r="R2" s="96" t="s">
         <v>783</v>
       </c>
-      <c r="R2" s="96" t="s">
+      <c r="S2" s="96" t="s">
         <v>784</v>
       </c>
-      <c r="S2" s="96" t="s">
+      <c r="T2" s="96" t="s">
         <v>785</v>
       </c>
-      <c r="T2" s="96" t="s">
+      <c r="U2" s="96" t="s">
         <v>786</v>
       </c>
-      <c r="U2" s="96" t="s">
+      <c r="V2" s="96" t="s">
         <v>787</v>
       </c>
-      <c r="V2" s="96" t="s">
+      <c r="W2" s="96" t="s">
         <v>788</v>
       </c>
-      <c r="W2" s="96" t="s">
+      <c r="X2" s="96" t="s">
         <v>789</v>
       </c>
-      <c r="X2" s="96" t="s">
+      <c r="Y2" s="96" t="s">
         <v>790</v>
       </c>
-      <c r="Y2" s="96" t="s">
+      <c r="Z2" s="96" t="s">
         <v>791</v>
-      </c>
-      <c r="Z2" s="96" t="s">
-        <v>792</v>
       </c>
       <c r="AA2" s="96" t="s">
         <v>61</v>
       </c>
       <c r="AB2" s="96" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="AC2" s="95" t="s">
         <v>255</v>
@@ -45562,7 +45565,7 @@
   <sheetData>
     <row r="1" spans="1:81" ht="185" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -45588,13 +45591,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="24" t="s">
+        <v>794</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>795</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>796</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>797</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>255</v>
@@ -46847,9 +46850,11 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1F6A15-066C-494D-992B-F6A4A794D67F}">
-  <dimension ref="A1:AN50"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -47017,16 +47022,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F2" s="44" t="s">
         <v>19</v>
@@ -47044,13 +47049,13 @@
         <v>42</v>
       </c>
       <c r="K2" s="44" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L2" s="44" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N2" s="44" t="s">
         <v>376</v>
@@ -47071,10 +47076,10 @@
         <v>237</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U2" s="44" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="V2" s="44" t="s">
         <v>414</v>
@@ -47139,16 +47144,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F3" s="44" t="s">
         <v>20</v>
@@ -47189,7 +47194,7 @@
         <v>417</v>
       </c>
       <c r="T3" s="44" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U3" s="44"/>
       <c r="V3" s="44" t="s">
@@ -47255,16 +47260,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" t="s">
@@ -47295,7 +47300,7 @@
         <v>421</v>
       </c>
       <c r="T4" s="44" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="U4" s="44"/>
       <c r="V4" s="44"/>
@@ -47341,10 +47346,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F5" s="44"/>
       <c r="G5" t="s">
@@ -47398,10 +47403,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" t="s">
@@ -47450,7 +47455,7 @@
         <v>533</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" t="s">
@@ -47494,10 +47499,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" t="s">
@@ -47541,10 +47546,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" t="s">
@@ -47588,10 +47593,10 @@
         <v>11</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" t="s">
@@ -47635,10 +47640,10 @@
         <v>12</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F11" s="44"/>
       <c r="G11" t="s">
@@ -47956,7 +47961,7 @@
       </c>
       <c r="F19" s="44"/>
       <c r="G19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H19" s="44"/>
       <c r="I19" s="44"/>
@@ -48346,7 +48351,7 @@
       </c>
       <c r="F29" s="44"/>
       <c r="G29" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="H29" s="44"/>
       <c r="I29" s="44"/>
@@ -48697,7 +48702,7 @@
       </c>
       <c r="F38" s="44"/>
       <c r="G38" t="s">
-        <v>559</v>
+        <v>797</v>
       </c>
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
@@ -48731,12 +48736,9 @@
       <c r="AI38" s="44"/>
     </row>
     <row r="39" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="43">
-        <v>40</v>
-      </c>
       <c r="F39" s="44"/>
       <c r="G39" t="s">
-        <v>560</v>
+        <v>798</v>
       </c>
       <c r="H39" s="44"/>
       <c r="I39" s="44"/>
@@ -48761,9 +48763,7 @@
       <c r="AB39" s="44"/>
       <c r="AC39" s="44"/>
       <c r="AD39" s="44"/>
-      <c r="AE39" s="44" t="s">
-        <v>195</v>
-      </c>
+      <c r="AE39" s="44"/>
       <c r="AF39" s="47"/>
       <c r="AG39" s="44"/>
       <c r="AH39" s="44"/>
@@ -48771,11 +48771,11 @@
     </row>
     <row r="40" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F40" s="44"/>
       <c r="G40" t="s">
-        <v>437</v>
+        <v>559</v>
       </c>
       <c r="H40" s="44"/>
       <c r="I40" s="44"/>
@@ -48797,10 +48797,11 @@
       <c r="Y40" s="44"/>
       <c r="Z40" s="44"/>
       <c r="AA40" s="44"/>
+      <c r="AB40" s="44"/>
       <c r="AC40" s="44"/>
       <c r="AD40" s="44"/>
       <c r="AE40" s="44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AF40" s="47"/>
       <c r="AG40" s="44"/>
@@ -48809,35 +48810,61 @@
     </row>
     <row r="41" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="43">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F41" s="44"/>
       <c r="G41" t="s">
-        <v>438</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
       <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
       <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
       <c r="T41" s="44"/>
       <c r="U41" s="44"/>
-      <c r="AF41" s="48"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="44"/>
+      <c r="AA41" s="44"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="44"/>
+      <c r="AE41" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF41" s="47"/>
+      <c r="AG41" s="44"/>
+      <c r="AH41" s="44"/>
+      <c r="AI41" s="44"/>
     </row>
     <row r="42" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G42" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K42" s="44"/>
       <c r="M42" s="44"/>
       <c r="T42" s="44"/>
       <c r="U42" s="44"/>
+      <c r="AF42" s="48"/>
     </row>
     <row r="43" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="43">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G43" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="K43" s="44"/>
       <c r="M43" s="44"/>
@@ -48846,10 +48873,10 @@
     </row>
     <row r="44" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="43">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G44" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K44" s="44"/>
       <c r="M44" s="44"/>
@@ -48858,7 +48885,10 @@
     </row>
     <row r="45" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="43">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="G45" t="s">
+        <v>441</v>
       </c>
       <c r="K45" s="44"/>
       <c r="M45" s="44"/>
@@ -48867,7 +48897,7 @@
     </row>
     <row r="46" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="43">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K46" s="44"/>
       <c r="M46" s="44"/>
@@ -48876,7 +48906,7 @@
     </row>
     <row r="47" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="43">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K47" s="44"/>
       <c r="M47" s="44"/>
@@ -48885,7 +48915,7 @@
     </row>
     <row r="48" spans="1:35" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="43">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K48" s="44"/>
       <c r="M48" s="44"/>
@@ -48894,7 +48924,7 @@
     </row>
     <row r="49" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="43">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K49" s="44"/>
       <c r="M49" s="44"/>
@@ -48902,7 +48932,16 @@
       <c r="U49" s="44"/>
     </row>
     <row r="50" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AB50" s="49"/>
+      <c r="A50" s="43">
+        <v>50</v>
+      </c>
+      <c r="K50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="T50" s="44"/>
+      <c r="U50" s="44"/>
+    </row>
+    <row r="51" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB51" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50090,7 +50129,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -50098,7 +50137,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -50106,7 +50145,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -50114,7 +50153,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -50415,7 +50454,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="30" customFormat="1" ht="131.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -50434,10 +50473,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>255</v>
@@ -52020,7 +52059,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="30" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -54380,7 +54419,7 @@
       <c r="E1" s="104"/>
       <c r="F1" s="105"/>
       <c r="G1" s="106" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="H1" s="107"/>
       <c r="I1" s="108"/>
@@ -54452,7 +54491,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="30" customFormat="1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B1" s="99"/>
       <c r="C1" s="99"/>
@@ -54470,7 +54509,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E2" s="74" t="s">
         <v>255</v>
@@ -54527,7 +54566,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="30" customFormat="1" ht="207" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="99" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B1" s="101"/>
       <c r="C1" s="101"/>
@@ -54554,34 +54593,34 @@
         <v>2</v>
       </c>
       <c r="D2" s="73" t="s">
+        <v>684</v>
+      </c>
+      <c r="E2" s="74" t="s">
         <v>685</v>
       </c>
-      <c r="E2" s="74" t="s">
+      <c r="F2" s="74" t="s">
         <v>686</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="G2" s="74" t="s">
         <v>687</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="H2" s="75" t="s">
         <v>688</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="I2" s="76" t="s">
         <v>689</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="J2" s="76" t="s">
         <v>690</v>
       </c>
-      <c r="J2" s="76" t="s">
+      <c r="K2" s="74" t="s">
         <v>691</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="L2" s="74" t="s">
         <v>692</v>
       </c>
-      <c r="L2" s="74" t="s">
+      <c r="M2" s="74" t="s">
         <v>693</v>
-      </c>
-      <c r="M2" s="74" t="s">
-        <v>694</v>
       </c>
       <c r="N2" s="77" t="s">
         <v>255</v>

</xml_diff>